<commit_message>
Marked column red those should not be overloaded in NewOrder sheet.
</commit_message>
<xml_diff>
--- a/SparkAutomation/src/Data/InputData.xlsx
+++ b/SparkAutomation/src/Data/InputData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="New_Order" sheetId="1" r:id="rId1"/>
@@ -852,8 +852,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,7 +877,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,8 +896,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -920,11 +926,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -946,6 +963,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,6 +1065,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1072,6 +1100,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1247,29 +1276,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:GF9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:GF10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="18" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="18" customWidth="1"/>
     <col min="15" max="15" width="34" customWidth="1"/>
     <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -1277,11 +1306,11 @@
     <col min="19" max="19" width="22.5703125" customWidth="1"/>
     <col min="20" max="20" width="17.5703125" customWidth="1"/>
     <col min="21" max="21" width="24.42578125" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
-    <col min="26" max="26" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="18" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" style="18" customWidth="1"/>
     <col min="27" max="27" width="25" customWidth="1"/>
     <col min="28" max="28" width="23.28515625" customWidth="1"/>
     <col min="29" max="29" width="22.140625" customWidth="1"/>
@@ -1299,7 +1328,9 @@
     <col min="50" max="50" width="23.5703125" customWidth="1"/>
     <col min="51" max="71" width="20.85546875" customWidth="1"/>
     <col min="72" max="72" width="24.5703125" customWidth="1"/>
-    <col min="73" max="78" width="20.85546875" customWidth="1"/>
+    <col min="73" max="74" width="20.85546875" customWidth="1"/>
+    <col min="75" max="75" width="20.85546875" style="18" customWidth="1"/>
+    <col min="76" max="78" width="20.85546875" customWidth="1"/>
     <col min="79" max="79" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1341,7 +1372,7 @@
     <col min="182" max="182" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188">
+    <row r="1" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>80</v>
       </c>
@@ -1469,7 +1500,7 @@
       <c r="DS1" s="4"/>
       <c r="DT1" s="4"/>
     </row>
-    <row r="2" spans="1:188" ht="30">
+    <row r="2" spans="1:188" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1479,37 +1510,37 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="15" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -1533,19 +1564,19 @@
       <c r="U2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="15" t="s">
         <v>103</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -1692,7 +1723,7 @@
       <c r="BV2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BW2" s="15" t="s">
         <v>144</v>
       </c>
       <c r="BX2" s="1" t="s">
@@ -2015,7 +2046,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:188" ht="16.5" customHeight="1">
+    <row r="3" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>169</v>
       </c>
@@ -2025,37 +2056,37 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="16">
         <v>4159381</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="19">
         <v>26121804</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="21" t="s">
         <v>151</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -2079,19 +2110,19 @@
       <c r="U3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="19">
         <v>12</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="19" t="s">
         <v>4</v>
       </c>
       <c r="AA3" s="4">
@@ -2150,7 +2181,7 @@
       <c r="BT3" s="4"/>
       <c r="BU3" s="4"/>
       <c r="BV3" s="4"/>
-      <c r="BW3" s="5" t="s">
+      <c r="BW3" s="21" t="s">
         <v>149</v>
       </c>
       <c r="BX3" s="5" t="s">
@@ -2269,7 +2300,7 @@
       <c r="DS3" s="4"/>
       <c r="DT3" s="4"/>
     </row>
-    <row r="4" spans="1:188">
+    <row r="4" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>170</v>
       </c>
@@ -2279,37 +2310,37 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="16">
         <v>4159381</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="19">
         <v>26121804</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="21" t="s">
         <v>151</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -2333,19 +2364,19 @@
       <c r="U4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="21">
         <v>12</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="21" t="s">
         <v>4</v>
       </c>
       <c r="AA4" s="3" t="s">
@@ -2404,7 +2435,7 @@
       <c r="BT4" s="4"/>
       <c r="BU4" s="4"/>
       <c r="BV4" s="4"/>
-      <c r="BW4" s="5" t="s">
+      <c r="BW4" s="21" t="s">
         <v>153</v>
       </c>
       <c r="BX4" s="5" t="s">
@@ -2493,7 +2524,7 @@
       <c r="DS4" s="4"/>
       <c r="DT4" s="4"/>
     </row>
-    <row r="5" spans="1:188" ht="16.5" customHeight="1">
+    <row r="5" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>171</v>
       </c>
@@ -2503,37 +2534,37 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="16">
         <v>4159381</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="19">
         <v>26121804</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="16" t="s">
         <v>151</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -2557,19 +2588,19 @@
       <c r="U5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="V5" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="X5" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="19">
         <v>1</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="Z5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="AA5" s="3">
@@ -2628,7 +2659,7 @@
       <c r="BT5" s="4"/>
       <c r="BU5" s="4"/>
       <c r="BV5" s="4"/>
-      <c r="BW5" s="8" t="s">
+      <c r="BW5" s="22" t="s">
         <v>167</v>
       </c>
       <c r="BX5" s="8" t="s">
@@ -2689,7 +2720,7 @@
       <c r="DS5" s="4"/>
       <c r="DT5" s="4"/>
     </row>
-    <row r="6" spans="1:188">
+    <row r="6" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>172</v>
       </c>
@@ -2699,37 +2730,37 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="16">
         <v>4159381</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="19">
         <v>26121804</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="16" t="s">
         <v>151</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -2753,19 +2784,19 @@
       <c r="U6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="V6" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="19">
         <v>1</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="Z6" s="19" t="s">
         <v>4</v>
       </c>
       <c r="AA6" s="3">
@@ -2824,7 +2855,7 @@
       <c r="BT6" s="4"/>
       <c r="BU6" s="4"/>
       <c r="BV6" s="4"/>
-      <c r="BW6" s="4" t="s">
+      <c r="BW6" s="19" t="s">
         <v>167</v>
       </c>
       <c r="BX6" s="4" t="s">
@@ -2885,7 +2916,7 @@
       <c r="DS6" s="4"/>
       <c r="DT6" s="4"/>
     </row>
-    <row r="7" spans="1:188" ht="16.5" customHeight="1">
+    <row r="7" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>200</v>
       </c>
@@ -2895,37 +2926,37 @@
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="16">
         <v>4159381</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="19">
         <v>26121804</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="21" t="s">
         <v>175</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -2949,19 +2980,19 @@
       <c r="U7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="19">
         <v>12</v>
       </c>
-      <c r="Z7" s="4" t="s">
+      <c r="Z7" s="19" t="s">
         <v>4</v>
       </c>
       <c r="AA7" s="4">
@@ -3086,7 +3117,7 @@
       <c r="BV7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="BW7" s="5" t="s">
+      <c r="BW7" s="21" t="s">
         <v>173</v>
       </c>
       <c r="BX7" s="5" t="s">
@@ -3219,7 +3250,7 @@
       <c r="DS7" s="4"/>
       <c r="DT7" s="4"/>
     </row>
-    <row r="8" spans="1:188">
+    <row r="8" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>201</v>
       </c>
@@ -3229,37 +3260,37 @@
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="16">
         <v>4159381</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="19">
         <v>26121804</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="19"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -3267,11 +3298,11 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
@@ -3322,7 +3353,7 @@
       <c r="BT8" s="4"/>
       <c r="BU8" s="4"/>
       <c r="BV8" s="4"/>
-      <c r="BW8" s="4"/>
+      <c r="BW8" s="19"/>
       <c r="BX8" s="4"/>
       <c r="BY8" s="4"/>
       <c r="BZ8" s="4" t="s">
@@ -3519,7 +3550,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:188">
+    <row r="9" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>271</v>
       </c>
@@ -3529,37 +3560,37 @@
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="16">
         <v>4159381</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="19">
         <v>26121804</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="16" t="s">
         <v>151</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -3583,19 +3614,19 @@
       <c r="U9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="V9" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="W9" s="5" t="s">
+      <c r="W9" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="X9" s="5" t="s">
+      <c r="X9" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="19">
         <v>1</v>
       </c>
-      <c r="Z9" s="4" t="s">
+      <c r="Z9" s="19" t="s">
         <v>4</v>
       </c>
       <c r="AA9" s="3">
@@ -3654,7 +3685,7 @@
       <c r="BT9" s="4"/>
       <c r="BU9" s="4"/>
       <c r="BV9" s="4"/>
-      <c r="BW9" s="5" t="s">
+      <c r="BW9" s="21" t="s">
         <v>272</v>
       </c>
       <c r="BX9" s="5" t="s">
@@ -3673,6 +3704,89 @@
       <c r="CE9" s="5" t="s">
         <v>272</v>
       </c>
+    </row>
+    <row r="10" spans="1:188" x14ac:dyDescent="0.25">
+      <c r="D10" s="17"/>
+      <c r="E10" s="20"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="20"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="20"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="14"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="14"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="20"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="14"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="14"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="14"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="14"/>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="14"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="14"/>
+      <c r="AZ10" s="13"/>
+      <c r="BA10" s="14"/>
+      <c r="BD10" s="13"/>
+      <c r="BE10" s="14"/>
+      <c r="BH10" s="13"/>
+      <c r="BI10" s="14"/>
+      <c r="BL10" s="13"/>
+      <c r="BM10" s="14"/>
+      <c r="BP10" s="13"/>
+      <c r="BQ10" s="14"/>
+      <c r="BT10" s="13"/>
+      <c r="BU10" s="14"/>
+      <c r="BX10" s="13"/>
+      <c r="BY10" s="14"/>
+      <c r="CB10" s="13"/>
+      <c r="CC10" s="14"/>
+      <c r="CF10" s="13"/>
+      <c r="CG10" s="14"/>
+      <c r="CJ10" s="13"/>
+      <c r="CK10" s="14"/>
+      <c r="CN10" s="13"/>
+      <c r="CO10" s="14"/>
+      <c r="CR10" s="13"/>
+      <c r="CS10" s="14"/>
+      <c r="CV10" s="13"/>
+      <c r="CW10" s="14"/>
+      <c r="CZ10" s="13"/>
+      <c r="DA10" s="14"/>
+      <c r="DD10" s="13"/>
+      <c r="DE10" s="14"/>
+      <c r="DH10" s="13"/>
+      <c r="DI10" s="14"/>
+      <c r="DL10" s="13"/>
+      <c r="DM10" s="14"/>
+      <c r="DP10" s="13"/>
+      <c r="DQ10" s="14"/>
+      <c r="DT10" s="13"/>
+      <c r="DU10" s="14"/>
+      <c r="DX10" s="13"/>
+      <c r="DY10" s="14"/>
+      <c r="EB10" s="13"/>
+      <c r="EC10" s="14"/>
+      <c r="EF10" s="13"/>
+      <c r="EG10" s="14"/>
+      <c r="EJ10" s="13"/>
+      <c r="EK10" s="14"/>
+      <c r="EN10" s="13"/>
+      <c r="EO10" s="14"/>
+      <c r="ER10" s="13"/>
+      <c r="ES10" s="14"/>
+      <c r="EV10" s="13"/>
+      <c r="EW10" s="14"/>
+      <c r="EZ10" s="13"/>
+      <c r="FA10" s="14"/>
+      <c r="FD10" s="13"/>
+      <c r="FE10" s="14"/>
+      <c r="FH10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3687,14 +3801,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -3781,7 +3895,7 @@
     <col min="182" max="182" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188">
+    <row r="1" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>80</v>
       </c>
@@ -3909,7 +4023,7 @@
       <c r="DS1" s="4"/>
       <c r="DT1" s="4"/>
     </row>
-    <row r="2" spans="1:188" ht="30">
+    <row r="2" spans="1:188" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4455,7 +4569,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:188" ht="16.5" customHeight="1">
+    <row r="3" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>169</v>
       </c>
@@ -4709,7 +4823,7 @@
       <c r="DS3" s="4"/>
       <c r="DT3" s="4"/>
     </row>
-    <row r="4" spans="1:188">
+    <row r="4" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>170</v>
       </c>
@@ -4933,7 +5047,7 @@
       <c r="DS4" s="4"/>
       <c r="DT4" s="4"/>
     </row>
-    <row r="5" spans="1:188" ht="16.5" customHeight="1">
+    <row r="5" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>171</v>
       </c>
@@ -5129,7 +5243,7 @@
       <c r="DS5" s="4"/>
       <c r="DT5" s="4"/>
     </row>
-    <row r="6" spans="1:188">
+    <row r="6" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>172</v>
       </c>
@@ -5325,7 +5439,7 @@
       <c r="DS6" s="4"/>
       <c r="DT6" s="4"/>
     </row>
-    <row r="7" spans="1:188" ht="16.5" customHeight="1">
+    <row r="7" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>200</v>
       </c>
@@ -5659,7 +5773,7 @@
       <c r="DS7" s="4"/>
       <c r="DT7" s="4"/>
     </row>
-    <row r="8" spans="1:188">
+    <row r="8" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>201</v>
       </c>
@@ -5959,7 +6073,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:188">
+    <row r="9" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>271</v>
       </c>
@@ -6124,14 +6238,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF9"/>
   <sheetViews>
     <sheetView topLeftCell="FI1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A1:FZ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -6218,7 +6332,7 @@
     <col min="182" max="182" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188">
+    <row r="1" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>80</v>
       </c>
@@ -6346,7 +6460,7 @@
       <c r="DS1" s="4"/>
       <c r="DT1" s="4"/>
     </row>
-    <row r="2" spans="1:188" ht="30">
+    <row r="2" spans="1:188" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6892,7 +7006,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:188" ht="16.5" customHeight="1">
+    <row r="3" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>169</v>
       </c>
@@ -7146,7 +7260,7 @@
       <c r="DS3" s="4"/>
       <c r="DT3" s="4"/>
     </row>
-    <row r="4" spans="1:188">
+    <row r="4" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>170</v>
       </c>
@@ -7370,7 +7484,7 @@
       <c r="DS4" s="4"/>
       <c r="DT4" s="4"/>
     </row>
-    <row r="5" spans="1:188" ht="16.5" customHeight="1">
+    <row r="5" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>171</v>
       </c>
@@ -7566,7 +7680,7 @@
       <c r="DS5" s="4"/>
       <c r="DT5" s="4"/>
     </row>
-    <row r="6" spans="1:188">
+    <row r="6" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>172</v>
       </c>
@@ -7762,7 +7876,7 @@
       <c r="DS6" s="4"/>
       <c r="DT6" s="4"/>
     </row>
-    <row r="7" spans="1:188" ht="16.5" customHeight="1">
+    <row r="7" spans="1:188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>200</v>
       </c>
@@ -8096,7 +8210,7 @@
       <c r="DS7" s="4"/>
       <c r="DT7" s="4"/>
     </row>
-    <row r="8" spans="1:188">
+    <row r="8" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>201</v>
       </c>
@@ -8396,7 +8510,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:188">
+    <row r="9" spans="1:188" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>271</v>
       </c>
@@ -8561,14 +8675,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:FZ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -8605,7 +8719,7 @@
     <col min="36" max="36" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:182">
+    <row r="1" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>80</v>
       </c>
@@ -8733,7 +8847,7 @@
       <c r="DS1" s="4"/>
       <c r="DT1" s="4"/>
     </row>
-    <row r="2" spans="1:182" ht="60">
+    <row r="2" spans="1:182" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -9279,7 +9393,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:182" ht="45">
+    <row r="3" spans="1:182" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>169</v>
       </c>
@@ -9533,7 +9647,7 @@
       <c r="DS3" s="4"/>
       <c r="DT3" s="4"/>
     </row>
-    <row r="4" spans="1:182" ht="45">
+    <row r="4" spans="1:182" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>170</v>
       </c>
@@ -9757,7 +9871,7 @@
       <c r="DS4" s="4"/>
       <c r="DT4" s="4"/>
     </row>
-    <row r="5" spans="1:182">
+    <row r="5" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>171</v>
       </c>
@@ -9953,7 +10067,7 @@
       <c r="DS5" s="4"/>
       <c r="DT5" s="4"/>
     </row>
-    <row r="6" spans="1:182">
+    <row r="6" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>172</v>
       </c>
@@ -10149,7 +10263,7 @@
       <c r="DS6" s="4"/>
       <c r="DT6" s="4"/>
     </row>
-    <row r="7" spans="1:182" ht="90">
+    <row r="7" spans="1:182" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>200</v>
       </c>
@@ -10483,7 +10597,7 @@
       <c r="DS7" s="4"/>
       <c r="DT7" s="4"/>
     </row>
-    <row r="8" spans="1:182">
+    <row r="8" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>201</v>
       </c>
@@ -10779,7 +10893,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:182">
+    <row r="9" spans="1:182" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>271</v>
       </c>

</xml_diff>

<commit_message>
Marked column red for cease and cancel those should not be overloaded in InputData.xlsx sheet
</commit_message>
<xml_diff>
--- a/SparkAutomation/src/Data/InputData.xlsx
+++ b/SparkAutomation/src/Data/InputData.xlsx
@@ -960,9 +960,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -973,6 +970,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1280,7 +1280,7 @@
   <dimension ref="A1:GF10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,17 +1288,17 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" style="18" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="17" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="17" customWidth="1"/>
     <col min="15" max="15" width="34" customWidth="1"/>
     <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -1306,11 +1306,11 @@
     <col min="19" max="19" width="22.5703125" customWidth="1"/>
     <col min="20" max="20" width="17.5703125" customWidth="1"/>
     <col min="21" max="21" width="24.42578125" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" style="18" customWidth="1"/>
-    <col min="26" max="26" width="22.5703125" style="18" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="17" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" style="17" customWidth="1"/>
     <col min="27" max="27" width="25" customWidth="1"/>
     <col min="28" max="28" width="23.28515625" customWidth="1"/>
     <col min="29" max="29" width="22.140625" customWidth="1"/>
@@ -1329,8 +1329,8 @@
     <col min="51" max="71" width="20.85546875" customWidth="1"/>
     <col min="72" max="72" width="24.5703125" customWidth="1"/>
     <col min="73" max="74" width="20.85546875" customWidth="1"/>
-    <col min="75" max="75" width="20.85546875" style="18" customWidth="1"/>
-    <col min="76" max="78" width="20.85546875" customWidth="1"/>
+    <col min="75" max="77" width="20.85546875" style="17" customWidth="1"/>
+    <col min="78" max="78" width="20.85546875" customWidth="1"/>
     <col min="79" max="79" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1373,121 +1373,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:188" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="12"/>
-      <c r="CA1" s="12"/>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
-      <c r="DC1" s="12"/>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22"/>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22"/>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
+      <c r="CW1" s="22"/>
+      <c r="CX1" s="22"/>
+      <c r="CY1" s="22"/>
+      <c r="CZ1" s="22"/>
+      <c r="DA1" s="22"/>
+      <c r="DB1" s="22"/>
+      <c r="DC1" s="22"/>
+      <c r="DD1" s="22"/>
+      <c r="DE1" s="22"/>
+      <c r="DF1" s="22"/>
+      <c r="DG1" s="22"/>
+      <c r="DH1" s="22"/>
+      <c r="DI1" s="22"/>
       <c r="DJ1" s="4"/>
       <c r="DK1" s="4"/>
       <c r="DL1" s="4"/>
@@ -1510,37 +1510,37 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="14" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -1564,19 +1564,19 @@
       <c r="U2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="W2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="15" t="s">
+      <c r="X2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="15" t="s">
+      <c r="Y2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="15" t="s">
+      <c r="Z2" s="14" t="s">
         <v>103</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -1723,13 +1723,13 @@
       <c r="BV2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BW2" s="15" t="s">
+      <c r="BW2" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="BX2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="BY2" s="14" t="s">
         <v>146</v>
       </c>
       <c r="BZ2" s="1"/>
@@ -2056,37 +2056,37 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>4159381</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="18">
         <v>26121804</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>151</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -2110,19 +2110,19 @@
       <c r="U3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="21" t="s">
+      <c r="X3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="19">
+      <c r="Y3" s="18">
         <v>12</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="Z3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA3" s="4">
@@ -2181,13 +2181,13 @@
       <c r="BT3" s="4"/>
       <c r="BU3" s="4"/>
       <c r="BV3" s="4"/>
-      <c r="BW3" s="21" t="s">
+      <c r="BW3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="BX3" s="5" t="s">
+      <c r="BX3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="BY3" s="5" t="s">
+      <c r="BY3" s="20" t="s">
         <v>149</v>
       </c>
       <c r="BZ3" s="4"/>
@@ -2310,37 +2310,37 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>4159381</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="18">
         <v>26121804</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>151</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -2364,19 +2364,19 @@
       <c r="U4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="X4" s="21" t="s">
+      <c r="X4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="Y4" s="20">
         <v>12</v>
       </c>
-      <c r="Z4" s="21" t="s">
+      <c r="Z4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="AA4" s="3" t="s">
@@ -2435,13 +2435,13 @@
       <c r="BT4" s="4"/>
       <c r="BU4" s="4"/>
       <c r="BV4" s="4"/>
-      <c r="BW4" s="21" t="s">
+      <c r="BW4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="BX4" s="5" t="s">
+      <c r="BX4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="BY4" s="5" t="s">
+      <c r="BY4" s="20" t="s">
         <v>153</v>
       </c>
       <c r="BZ4" s="5" t="s">
@@ -2534,37 +2534,37 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>4159381</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>26121804</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -2588,19 +2588,19 @@
       <c r="U5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X5" s="22" t="s">
+      <c r="X5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="18">
         <v>1</v>
       </c>
-      <c r="Z5" s="19" t="s">
+      <c r="Z5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA5" s="3">
@@ -2659,13 +2659,13 @@
       <c r="BT5" s="4"/>
       <c r="BU5" s="4"/>
       <c r="BV5" s="4"/>
-      <c r="BW5" s="22" t="s">
+      <c r="BW5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BX5" s="8" t="s">
+      <c r="BX5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BY5" s="8" t="s">
+      <c r="BY5" s="21" t="s">
         <v>167</v>
       </c>
       <c r="BZ5" s="4"/>
@@ -2730,37 +2730,37 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>4159381</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="18">
         <v>26121804</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="N6" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -2784,19 +2784,19 @@
       <c r="U6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V6" s="22" t="s">
+      <c r="V6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="W6" s="22" t="s">
+      <c r="W6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X6" s="22" t="s">
+      <c r="X6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="18">
         <v>1</v>
       </c>
-      <c r="Z6" s="19" t="s">
+      <c r="Z6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA6" s="3">
@@ -2855,13 +2855,13 @@
       <c r="BT6" s="4"/>
       <c r="BU6" s="4"/>
       <c r="BV6" s="4"/>
-      <c r="BW6" s="19" t="s">
+      <c r="BW6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="BX6" s="4" t="s">
+      <c r="BX6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="BY6" s="4" t="s">
+      <c r="BY6" s="18" t="s">
         <v>167</v>
       </c>
       <c r="BZ6" s="4"/>
@@ -2926,37 +2926,37 @@
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>4159381</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>26121804</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="20" t="s">
         <v>175</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -2980,19 +2980,19 @@
       <c r="U7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="V7" s="21" t="s">
+      <c r="V7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="W7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="X7" s="21" t="s">
+      <c r="X7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="18">
         <v>12</v>
       </c>
-      <c r="Z7" s="19" t="s">
+      <c r="Z7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA7" s="4">
@@ -3117,13 +3117,13 @@
       <c r="BV7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="BW7" s="21" t="s">
+      <c r="BW7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BX7" s="5" t="s">
+      <c r="BX7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BY7" s="5" t="s">
+      <c r="BY7" s="20" t="s">
         <v>173</v>
       </c>
       <c r="BZ7" s="4" t="s">
@@ -3260,37 +3260,37 @@
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="15">
         <v>4159381</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="18">
         <v>26121804</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="19"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -3298,11 +3298,11 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
@@ -3353,9 +3353,9 @@
       <c r="BT8" s="4"/>
       <c r="BU8" s="4"/>
       <c r="BV8" s="4"/>
-      <c r="BW8" s="19"/>
-      <c r="BX8" s="4"/>
-      <c r="BY8" s="4"/>
+      <c r="BW8" s="18"/>
+      <c r="BX8" s="18"/>
+      <c r="BY8" s="18"/>
       <c r="BZ8" s="4" t="s">
         <v>201</v>
       </c>
@@ -3560,37 +3560,37 @@
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>4159381</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="18">
         <v>26121804</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="L9" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="16" t="s">
+      <c r="N9" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -3614,19 +3614,19 @@
       <c r="U9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V9" s="21" t="s">
+      <c r="V9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="W9" s="21" t="s">
+      <c r="W9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="X9" s="21" t="s">
+      <c r="X9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="Y9" s="19">
+      <c r="Y9" s="18">
         <v>1</v>
       </c>
-      <c r="Z9" s="19" t="s">
+      <c r="Z9" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA9" s="3">
@@ -3685,13 +3685,13 @@
       <c r="BT9" s="4"/>
       <c r="BU9" s="4"/>
       <c r="BV9" s="4"/>
-      <c r="BW9" s="21" t="s">
+      <c r="BW9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BX9" s="5" t="s">
+      <c r="BX9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BY9" s="5" t="s">
+      <c r="BY9" s="20" t="s">
         <v>272</v>
       </c>
       <c r="BZ9" s="4"/>
@@ -3706,87 +3706,87 @@
       </c>
     </row>
     <row r="10" spans="1:188" x14ac:dyDescent="0.25">
-      <c r="D10" s="17"/>
-      <c r="E10" s="20"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="20"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="20"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="14"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="14"/>
-      <c r="X10" s="17"/>
-      <c r="Y10" s="20"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="14"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="14"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="14"/>
-      <c r="AN10" s="13"/>
-      <c r="AO10" s="14"/>
-      <c r="AR10" s="13"/>
-      <c r="AS10" s="14"/>
-      <c r="AV10" s="13"/>
-      <c r="AW10" s="14"/>
-      <c r="AZ10" s="13"/>
-      <c r="BA10" s="14"/>
-      <c r="BD10" s="13"/>
-      <c r="BE10" s="14"/>
-      <c r="BH10" s="13"/>
-      <c r="BI10" s="14"/>
-      <c r="BL10" s="13"/>
-      <c r="BM10" s="14"/>
-      <c r="BP10" s="13"/>
-      <c r="BQ10" s="14"/>
-      <c r="BT10" s="13"/>
-      <c r="BU10" s="14"/>
-      <c r="BX10" s="13"/>
-      <c r="BY10" s="14"/>
-      <c r="CB10" s="13"/>
-      <c r="CC10" s="14"/>
-      <c r="CF10" s="13"/>
-      <c r="CG10" s="14"/>
-      <c r="CJ10" s="13"/>
-      <c r="CK10" s="14"/>
-      <c r="CN10" s="13"/>
-      <c r="CO10" s="14"/>
-      <c r="CR10" s="13"/>
-      <c r="CS10" s="14"/>
-      <c r="CV10" s="13"/>
-      <c r="CW10" s="14"/>
-      <c r="CZ10" s="13"/>
-      <c r="DA10" s="14"/>
-      <c r="DD10" s="13"/>
-      <c r="DE10" s="14"/>
-      <c r="DH10" s="13"/>
-      <c r="DI10" s="14"/>
-      <c r="DL10" s="13"/>
-      <c r="DM10" s="14"/>
-      <c r="DP10" s="13"/>
-      <c r="DQ10" s="14"/>
-      <c r="DT10" s="13"/>
-      <c r="DU10" s="14"/>
-      <c r="DX10" s="13"/>
-      <c r="DY10" s="14"/>
-      <c r="EB10" s="13"/>
-      <c r="EC10" s="14"/>
-      <c r="EF10" s="13"/>
-      <c r="EG10" s="14"/>
-      <c r="EJ10" s="13"/>
-      <c r="EK10" s="14"/>
-      <c r="EN10" s="13"/>
-      <c r="EO10" s="14"/>
-      <c r="ER10" s="13"/>
-      <c r="ES10" s="14"/>
-      <c r="EV10" s="13"/>
-      <c r="EW10" s="14"/>
-      <c r="EZ10" s="13"/>
-      <c r="FA10" s="14"/>
-      <c r="FD10" s="13"/>
-      <c r="FE10" s="14"/>
-      <c r="FH10" s="13"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="19"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="19"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="13"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="13"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="19"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="13"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="13"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="13"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="13"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="13"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="13"/>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="13"/>
+      <c r="BD10" s="12"/>
+      <c r="BE10" s="13"/>
+      <c r="BH10" s="12"/>
+      <c r="BI10" s="13"/>
+      <c r="BL10" s="12"/>
+      <c r="BM10" s="13"/>
+      <c r="BP10" s="12"/>
+      <c r="BQ10" s="13"/>
+      <c r="BT10" s="12"/>
+      <c r="BU10" s="13"/>
+      <c r="BX10" s="16"/>
+      <c r="BY10" s="19"/>
+      <c r="CB10" s="12"/>
+      <c r="CC10" s="13"/>
+      <c r="CF10" s="12"/>
+      <c r="CG10" s="13"/>
+      <c r="CJ10" s="12"/>
+      <c r="CK10" s="13"/>
+      <c r="CN10" s="12"/>
+      <c r="CO10" s="13"/>
+      <c r="CR10" s="12"/>
+      <c r="CS10" s="13"/>
+      <c r="CV10" s="12"/>
+      <c r="CW10" s="13"/>
+      <c r="CZ10" s="12"/>
+      <c r="DA10" s="13"/>
+      <c r="DD10" s="12"/>
+      <c r="DE10" s="13"/>
+      <c r="DH10" s="12"/>
+      <c r="DI10" s="13"/>
+      <c r="DL10" s="12"/>
+      <c r="DM10" s="13"/>
+      <c r="DP10" s="12"/>
+      <c r="DQ10" s="13"/>
+      <c r="DT10" s="12"/>
+      <c r="DU10" s="13"/>
+      <c r="DX10" s="12"/>
+      <c r="DY10" s="13"/>
+      <c r="EB10" s="12"/>
+      <c r="EC10" s="13"/>
+      <c r="EF10" s="12"/>
+      <c r="EG10" s="13"/>
+      <c r="EJ10" s="12"/>
+      <c r="EK10" s="13"/>
+      <c r="EN10" s="12"/>
+      <c r="EO10" s="13"/>
+      <c r="ER10" s="12"/>
+      <c r="ES10" s="13"/>
+      <c r="EV10" s="12"/>
+      <c r="EW10" s="13"/>
+      <c r="EZ10" s="12"/>
+      <c r="FA10" s="13"/>
+      <c r="FD10" s="12"/>
+      <c r="FE10" s="13"/>
+      <c r="FH10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3802,10 +3802,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GF9"/>
+  <dimension ref="A1:GF10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,17 +3813,17 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="17" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="17" customWidth="1"/>
     <col min="15" max="15" width="34" customWidth="1"/>
     <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -3831,11 +3831,11 @@
     <col min="19" max="19" width="22.5703125" customWidth="1"/>
     <col min="20" max="20" width="17.5703125" customWidth="1"/>
     <col min="21" max="21" width="24.42578125" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
-    <col min="26" max="26" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="17" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" style="17" customWidth="1"/>
     <col min="27" max="27" width="25" customWidth="1"/>
     <col min="28" max="28" width="23.28515625" customWidth="1"/>
     <col min="29" max="29" width="22.140625" customWidth="1"/>
@@ -3853,7 +3853,9 @@
     <col min="50" max="50" width="23.5703125" customWidth="1"/>
     <col min="51" max="71" width="20.85546875" customWidth="1"/>
     <col min="72" max="72" width="24.5703125" customWidth="1"/>
-    <col min="73" max="78" width="20.85546875" customWidth="1"/>
+    <col min="73" max="74" width="20.85546875" customWidth="1"/>
+    <col min="75" max="77" width="20.85546875" style="17" customWidth="1"/>
+    <col min="78" max="78" width="20.85546875" customWidth="1"/>
     <col min="79" max="79" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -3896,121 +3898,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:188" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="12"/>
-      <c r="CA1" s="12"/>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
-      <c r="DC1" s="12"/>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22"/>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22"/>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
+      <c r="CW1" s="22"/>
+      <c r="CX1" s="22"/>
+      <c r="CY1" s="22"/>
+      <c r="CZ1" s="22"/>
+      <c r="DA1" s="22"/>
+      <c r="DB1" s="22"/>
+      <c r="DC1" s="22"/>
+      <c r="DD1" s="22"/>
+      <c r="DE1" s="22"/>
+      <c r="DF1" s="22"/>
+      <c r="DG1" s="22"/>
+      <c r="DH1" s="22"/>
+      <c r="DI1" s="22"/>
       <c r="DJ1" s="4"/>
       <c r="DK1" s="4"/>
       <c r="DL1" s="4"/>
@@ -4033,37 +4035,37 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="14" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -4087,19 +4089,19 @@
       <c r="U2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="14" t="s">
         <v>103</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -4246,13 +4248,13 @@
       <c r="BV2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BW2" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="BX2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="BY2" s="14" t="s">
         <v>146</v>
       </c>
       <c r="BZ2" s="1"/>
@@ -4579,37 +4581,37 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="15">
         <v>4159381</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="18">
         <v>26121804</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="20" t="s">
         <v>151</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -4633,19 +4635,19 @@
       <c r="U3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="18">
         <v>12</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA3" s="4">
@@ -4704,13 +4706,13 @@
       <c r="BT3" s="4"/>
       <c r="BU3" s="4"/>
       <c r="BV3" s="4"/>
-      <c r="BW3" s="5" t="s">
+      <c r="BW3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="BX3" s="5" t="s">
+      <c r="BX3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="BY3" s="5" t="s">
+      <c r="BY3" s="20" t="s">
         <v>149</v>
       </c>
       <c r="BZ3" s="4"/>
@@ -4833,37 +4835,37 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="15">
         <v>4159381</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="18">
         <v>26121804</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="20" t="s">
         <v>151</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -4887,19 +4889,19 @@
       <c r="U4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="20">
         <v>12</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="AA4" s="3" t="s">
@@ -4958,13 +4960,13 @@
       <c r="BT4" s="4"/>
       <c r="BU4" s="4"/>
       <c r="BV4" s="4"/>
-      <c r="BW4" s="5" t="s">
+      <c r="BW4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="BX4" s="5" t="s">
+      <c r="BX4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="BY4" s="5" t="s">
+      <c r="BY4" s="20" t="s">
         <v>153</v>
       </c>
       <c r="BZ4" s="5" t="s">
@@ -5057,37 +5059,37 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="15">
         <v>4159381</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="18">
         <v>26121804</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -5111,19 +5113,19 @@
       <c r="U5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="V5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="X5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="18">
         <v>1</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="Z5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA5" s="3">
@@ -5182,13 +5184,13 @@
       <c r="BT5" s="4"/>
       <c r="BU5" s="4"/>
       <c r="BV5" s="4"/>
-      <c r="BW5" s="8" t="s">
+      <c r="BW5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BX5" s="8" t="s">
+      <c r="BX5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BY5" s="8" t="s">
+      <c r="BY5" s="21" t="s">
         <v>167</v>
       </c>
       <c r="BZ5" s="4"/>
@@ -5253,37 +5255,37 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="15">
         <v>4159381</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="18">
         <v>26121804</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -5307,19 +5309,19 @@
       <c r="U6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="V6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="18">
         <v>1</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="Z6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA6" s="3">
@@ -5378,13 +5380,13 @@
       <c r="BT6" s="4"/>
       <c r="BU6" s="4"/>
       <c r="BV6" s="4"/>
-      <c r="BW6" s="4" t="s">
+      <c r="BW6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="BX6" s="4" t="s">
+      <c r="BX6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="BY6" s="4" t="s">
+      <c r="BY6" s="18" t="s">
         <v>167</v>
       </c>
       <c r="BZ6" s="4"/>
@@ -5449,37 +5451,37 @@
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="15">
         <v>4159381</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="18">
         <v>26121804</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="20" t="s">
         <v>175</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -5503,19 +5505,19 @@
       <c r="U7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="18">
         <v>12</v>
       </c>
-      <c r="Z7" s="4" t="s">
+      <c r="Z7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA7" s="4">
@@ -5640,13 +5642,13 @@
       <c r="BV7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="BW7" s="5" t="s">
+      <c r="BW7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BX7" s="5" t="s">
+      <c r="BX7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BY7" s="5" t="s">
+      <c r="BY7" s="20" t="s">
         <v>173</v>
       </c>
       <c r="BZ7" s="4" t="s">
@@ -5783,37 +5785,37 @@
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="15">
         <v>4159381</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="18">
         <v>26121804</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -5821,11 +5823,11 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
@@ -5876,9 +5878,9 @@
       <c r="BT8" s="4"/>
       <c r="BU8" s="4"/>
       <c r="BV8" s="4"/>
-      <c r="BW8" s="4"/>
-      <c r="BX8" s="4"/>
-      <c r="BY8" s="4"/>
+      <c r="BW8" s="18"/>
+      <c r="BX8" s="18"/>
+      <c r="BY8" s="18"/>
       <c r="BZ8" s="4" t="s">
         <v>201</v>
       </c>
@@ -6083,37 +6085,37 @@
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="15">
         <v>4159381</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="18">
         <v>26121804</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -6137,19 +6139,19 @@
       <c r="U9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="V9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="W9" s="5" t="s">
+      <c r="W9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="X9" s="5" t="s">
+      <c r="X9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="18">
         <v>1</v>
       </c>
-      <c r="Z9" s="4" t="s">
+      <c r="Z9" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA9" s="3">
@@ -6208,13 +6210,13 @@
       <c r="BT9" s="4"/>
       <c r="BU9" s="4"/>
       <c r="BV9" s="4"/>
-      <c r="BW9" s="5" t="s">
+      <c r="BW9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BX9" s="5" t="s">
+      <c r="BX9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BY9" s="5" t="s">
+      <c r="BY9" s="20" t="s">
         <v>272</v>
       </c>
       <c r="BZ9" s="4"/>
@@ -6227,6 +6229,10 @@
       <c r="CE9" s="5" t="s">
         <v>272</v>
       </c>
+    </row>
+    <row r="10" spans="1:188" x14ac:dyDescent="0.25">
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6239,10 +6245,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GF9"/>
+  <dimension ref="A1:GF10"/>
   <sheetViews>
-    <sheetView topLeftCell="FI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:FZ9"/>
+    <sheetView topLeftCell="BU1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BU10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6250,17 +6256,17 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="17" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="17" customWidth="1"/>
     <col min="15" max="15" width="34" customWidth="1"/>
     <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -6268,11 +6274,11 @@
     <col min="19" max="19" width="22.5703125" customWidth="1"/>
     <col min="20" max="20" width="17.5703125" customWidth="1"/>
     <col min="21" max="21" width="24.42578125" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" customWidth="1"/>
-    <col min="26" max="26" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="17" customWidth="1"/>
+    <col min="26" max="26" width="22.5703125" style="17" customWidth="1"/>
     <col min="27" max="27" width="25" customWidth="1"/>
     <col min="28" max="28" width="23.28515625" customWidth="1"/>
     <col min="29" max="29" width="22.140625" customWidth="1"/>
@@ -6290,7 +6296,9 @@
     <col min="50" max="50" width="23.5703125" customWidth="1"/>
     <col min="51" max="71" width="20.85546875" customWidth="1"/>
     <col min="72" max="72" width="24.5703125" customWidth="1"/>
-    <col min="73" max="78" width="20.85546875" customWidth="1"/>
+    <col min="73" max="74" width="20.85546875" customWidth="1"/>
+    <col min="75" max="77" width="20.85546875" style="17" customWidth="1"/>
+    <col min="78" max="78" width="20.85546875" customWidth="1"/>
     <col min="79" max="79" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -6333,121 +6341,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:188" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="12"/>
-      <c r="CA1" s="12"/>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
-      <c r="DC1" s="12"/>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22"/>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22"/>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
+      <c r="CW1" s="22"/>
+      <c r="CX1" s="22"/>
+      <c r="CY1" s="22"/>
+      <c r="CZ1" s="22"/>
+      <c r="DA1" s="22"/>
+      <c r="DB1" s="22"/>
+      <c r="DC1" s="22"/>
+      <c r="DD1" s="22"/>
+      <c r="DE1" s="22"/>
+      <c r="DF1" s="22"/>
+      <c r="DG1" s="22"/>
+      <c r="DH1" s="22"/>
+      <c r="DI1" s="22"/>
       <c r="DJ1" s="4"/>
       <c r="DK1" s="4"/>
       <c r="DL1" s="4"/>
@@ -6470,37 +6478,37 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="14" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -6524,19 +6532,19 @@
       <c r="U2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="14" t="s">
         <v>103</v>
       </c>
       <c r="AA2" s="1" t="s">
@@ -6683,13 +6691,13 @@
       <c r="BV2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BW2" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="BX2" s="1" t="s">
+      <c r="BX2" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="BY2" s="14" t="s">
         <v>146</v>
       </c>
       <c r="BZ2" s="1"/>
@@ -7016,37 +7024,37 @@
       <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="15">
         <v>4159381</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="18">
         <v>26121804</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="20" t="s">
         <v>151</v>
       </c>
       <c r="O3" s="6" t="s">
@@ -7070,19 +7078,19 @@
       <c r="U3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="18">
         <v>12</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA3" s="4">
@@ -7141,13 +7149,13 @@
       <c r="BT3" s="4"/>
       <c r="BU3" s="4"/>
       <c r="BV3" s="4"/>
-      <c r="BW3" s="5" t="s">
+      <c r="BW3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="BX3" s="5" t="s">
+      <c r="BX3" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="BY3" s="5" t="s">
+      <c r="BY3" s="20" t="s">
         <v>149</v>
       </c>
       <c r="BZ3" s="4"/>
@@ -7270,37 +7278,37 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="15">
         <v>4159381</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="18">
         <v>26121804</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="20" t="s">
         <v>151</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -7324,19 +7332,19 @@
       <c r="U4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="X4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="20">
         <v>12</v>
       </c>
-      <c r="Z4" s="5" t="s">
+      <c r="Z4" s="20" t="s">
         <v>4</v>
       </c>
       <c r="AA4" s="3" t="s">
@@ -7395,13 +7403,13 @@
       <c r="BT4" s="4"/>
       <c r="BU4" s="4"/>
       <c r="BV4" s="4"/>
-      <c r="BW4" s="5" t="s">
+      <c r="BW4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="BX4" s="5" t="s">
+      <c r="BX4" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="BY4" s="5" t="s">
+      <c r="BY4" s="20" t="s">
         <v>153</v>
       </c>
       <c r="BZ4" s="5" t="s">
@@ -7494,37 +7502,37 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="15">
         <v>4159381</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="18">
         <v>26121804</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -7548,19 +7556,19 @@
       <c r="U5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V5" s="8" t="s">
+      <c r="V5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="W5" s="8" t="s">
+      <c r="W5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X5" s="8" t="s">
+      <c r="X5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="18">
         <v>1</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="Z5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA5" s="3">
@@ -7619,13 +7627,13 @@
       <c r="BT5" s="4"/>
       <c r="BU5" s="4"/>
       <c r="BV5" s="4"/>
-      <c r="BW5" s="8" t="s">
+      <c r="BW5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BX5" s="8" t="s">
+      <c r="BX5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="BY5" s="8" t="s">
+      <c r="BY5" s="21" t="s">
         <v>167</v>
       </c>
       <c r="BZ5" s="4"/>
@@ -7690,37 +7698,37 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="15">
         <v>4159381</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="18">
         <v>26121804</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -7744,19 +7752,19 @@
       <c r="U6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="V6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="X6" s="8" t="s">
+      <c r="X6" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="18">
         <v>1</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="Z6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA6" s="3">
@@ -7815,13 +7823,13 @@
       <c r="BT6" s="4"/>
       <c r="BU6" s="4"/>
       <c r="BV6" s="4"/>
-      <c r="BW6" s="4" t="s">
+      <c r="BW6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="BX6" s="4" t="s">
+      <c r="BX6" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="BY6" s="4" t="s">
+      <c r="BY6" s="18" t="s">
         <v>167</v>
       </c>
       <c r="BZ6" s="4"/>
@@ -7886,37 +7894,37 @@
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="15">
         <v>4159381</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="18">
         <v>26121804</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="20" t="s">
         <v>175</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -7940,19 +7948,19 @@
       <c r="U7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="18">
         <v>12</v>
       </c>
-      <c r="Z7" s="4" t="s">
+      <c r="Z7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA7" s="4">
@@ -8077,13 +8085,13 @@
       <c r="BV7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="BW7" s="5" t="s">
+      <c r="BW7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BX7" s="5" t="s">
+      <c r="BX7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BY7" s="5" t="s">
+      <c r="BY7" s="20" t="s">
         <v>173</v>
       </c>
       <c r="BZ7" s="4" t="s">
@@ -8220,37 +8228,37 @@
       <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="15">
         <v>4159381</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="18">
         <v>26121804</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -8258,11 +8266,11 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="4"/>
@@ -8313,9 +8321,9 @@
       <c r="BT8" s="4"/>
       <c r="BU8" s="4"/>
       <c r="BV8" s="4"/>
-      <c r="BW8" s="4"/>
-      <c r="BX8" s="4"/>
-      <c r="BY8" s="4"/>
+      <c r="BW8" s="18"/>
+      <c r="BX8" s="18"/>
+      <c r="BY8" s="18"/>
       <c r="BZ8" s="4" t="s">
         <v>201</v>
       </c>
@@ -8520,37 +8528,37 @@
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="15">
         <v>4159381</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="18">
         <v>26121804</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="15" t="s">
         <v>151</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -8574,19 +8582,19 @@
       <c r="U9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="V9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="W9" s="5" t="s">
+      <c r="W9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="X9" s="5" t="s">
+      <c r="X9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="18">
         <v>1</v>
       </c>
-      <c r="Z9" s="4" t="s">
+      <c r="Z9" s="18" t="s">
         <v>4</v>
       </c>
       <c r="AA9" s="3">
@@ -8645,13 +8653,13 @@
       <c r="BT9" s="4"/>
       <c r="BU9" s="4"/>
       <c r="BV9" s="4"/>
-      <c r="BW9" s="5" t="s">
+      <c r="BW9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BX9" s="5" t="s">
+      <c r="BX9" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="BY9" s="5" t="s">
+      <c r="BY9" s="20" t="s">
         <v>272</v>
       </c>
       <c r="BZ9" s="4"/>
@@ -8664,6 +8672,70 @@
       <c r="CE9" s="5" t="s">
         <v>272</v>
       </c>
+    </row>
+    <row r="10" spans="1:188" x14ac:dyDescent="0.25">
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="19"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="19"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="13"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="13"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="19"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="13"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="13"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="13"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="13"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="13"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="13"/>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="13"/>
+      <c r="BD10" s="12"/>
+      <c r="BE10" s="13"/>
+      <c r="BH10" s="12"/>
+      <c r="BI10" s="13"/>
+      <c r="BL10" s="12"/>
+      <c r="BM10" s="13"/>
+      <c r="BP10" s="12"/>
+      <c r="BQ10" s="13"/>
+      <c r="BT10" s="12"/>
+      <c r="BU10" s="13"/>
+      <c r="BX10" s="16"/>
+      <c r="BY10" s="19"/>
+      <c r="CB10" s="12"/>
+      <c r="CC10" s="13"/>
+      <c r="CF10" s="12"/>
+      <c r="CG10" s="13"/>
+      <c r="CJ10" s="12"/>
+      <c r="CK10" s="13"/>
+      <c r="CN10" s="12"/>
+      <c r="CO10" s="13"/>
+      <c r="CR10" s="12"/>
+      <c r="CS10" s="13"/>
+      <c r="CV10" s="12"/>
+      <c r="CW10" s="13"/>
+      <c r="CZ10" s="12"/>
+      <c r="DA10" s="13"/>
+      <c r="DD10" s="12"/>
+      <c r="DE10" s="13"/>
+      <c r="DH10" s="12"/>
+      <c r="DI10" s="13"/>
+      <c r="DL10" s="12"/>
+      <c r="DM10" s="13"/>
+      <c r="DP10" s="12"/>
+      <c r="DQ10" s="13"/>
+      <c r="DT10" s="12"/>
+      <c r="DU10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8720,121 +8792,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:182" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="12"/>
-      <c r="CA1" s="12"/>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="12"/>
-      <c r="DC1" s="12"/>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
+      <c r="AD1" s="22"/>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22"/>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="22"/>
+      <c r="BF1" s="22"/>
+      <c r="BG1" s="22"/>
+      <c r="BH1" s="22"/>
+      <c r="BI1" s="22"/>
+      <c r="BJ1" s="22"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
+      <c r="BM1" s="22"/>
+      <c r="BN1" s="22"/>
+      <c r="BO1" s="22"/>
+      <c r="BP1" s="22"/>
+      <c r="BQ1" s="22"/>
+      <c r="BR1" s="22"/>
+      <c r="BS1" s="22"/>
+      <c r="BT1" s="22"/>
+      <c r="BU1" s="22"/>
+      <c r="BV1" s="22"/>
+      <c r="BW1" s="22"/>
+      <c r="BX1" s="22"/>
+      <c r="BY1" s="22"/>
+      <c r="BZ1" s="22"/>
+      <c r="CA1" s="22"/>
+      <c r="CB1" s="22"/>
+      <c r="CC1" s="22"/>
+      <c r="CD1" s="22"/>
+      <c r="CE1" s="22"/>
+      <c r="CF1" s="22"/>
+      <c r="CG1" s="22"/>
+      <c r="CH1" s="22"/>
+      <c r="CI1" s="22"/>
+      <c r="CJ1" s="22"/>
+      <c r="CK1" s="22"/>
+      <c r="CL1" s="22"/>
+      <c r="CM1" s="22"/>
+      <c r="CN1" s="22"/>
+      <c r="CO1" s="22"/>
+      <c r="CP1" s="22"/>
+      <c r="CQ1" s="22"/>
+      <c r="CR1" s="22"/>
+      <c r="CS1" s="22"/>
+      <c r="CT1" s="22"/>
+      <c r="CU1" s="22"/>
+      <c r="CV1" s="22"/>
+      <c r="CW1" s="22"/>
+      <c r="CX1" s="22"/>
+      <c r="CY1" s="22"/>
+      <c r="CZ1" s="22"/>
+      <c r="DA1" s="22"/>
+      <c r="DB1" s="22"/>
+      <c r="DC1" s="22"/>
+      <c r="DD1" s="22"/>
+      <c r="DE1" s="22"/>
+      <c r="DF1" s="22"/>
+      <c r="DG1" s="22"/>
+      <c r="DH1" s="22"/>
+      <c r="DI1" s="22"/>
       <c r="DJ1" s="4"/>
       <c r="DK1" s="4"/>
       <c r="DL1" s="4"/>

</xml_diff>